<commit_message>
get, get all, put and delete
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sqasa1-my.sharepoint.com/personal/luis_estrada_sqasa_co/Documents/Documentos Personales/Retos/RetoTecnicoChoucair/RetoTecnologiaAPIs/src/main/resources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60769EA-22AD-4677-98CB-84489788D05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{D60769EA-22AD-4677-98CB-84489788D05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E94F7C92-5DBB-47A8-8182-D7CE8C0651FC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -45,13 +45,67 @@
     <t>felipe</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
     <t>Successfully! Record has been added.</t>
+  </si>
+  <si>
+    <t>/employee/</t>
+  </si>
+  <si>
+    <t>endPointGet</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Successfully! Record has been fetched.</t>
+  </si>
+  <si>
+    <t>messageGet</t>
+  </si>
+  <si>
+    <t>messagePost</t>
+  </si>
+  <si>
+    <t>endPointPut</t>
+  </si>
+  <si>
+    <t>nameUpdate</t>
+  </si>
+  <si>
+    <t>salaryUpdate</t>
+  </si>
+  <si>
+    <t>ageUpdate</t>
+  </si>
+  <si>
+    <t>Successfully! Record has been updated.</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>/update/</t>
+  </si>
+  <si>
+    <t>endPointDelete</t>
+  </si>
+  <si>
+    <t>messageDelete</t>
+  </si>
+  <si>
+    <t>Successfully! Record has been deleted</t>
+  </si>
+  <si>
+    <t>/delete/</t>
+  </si>
+  <si>
+    <t>endPointGetAll</t>
+  </si>
+  <si>
+    <t>/employees</t>
+  </si>
+  <si>
+    <t>Successfully! All records has been fetched.</t>
   </si>
 </sst>
 </file>
@@ -67,15 +121,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,13 +155,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -105,6 +198,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,47 +479,125 @@
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
+        <v>200</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2">
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="N2" s="1">
         <v>30</v>
       </c>
-      <c r="E2">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="O2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>